<commit_message>
Fixed opening position of web export reports and updated the metadata.
</commit_message>
<xml_diff>
--- a/db/reports/hui-south-maui-thru-2019-1st-quarter.0.xlsx
+++ b/db/reports/hui-south-maui-thru-2019-1st-quarter.0.xlsx
@@ -2404,8 +2404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A470" workbookViewId="0">
-      <selection activeCell="X506" sqref="X506"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O498" sqref="O498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -36478,7 +36478,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -36510,7 +36510,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3">
-        <v>43193</v>
+        <v>43618</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>

</xml_diff>